<commit_message>
bug fix for recruit solder
</commit_message>
<xml_diff>
--- a/gameData/shared/HouseFunction.xlsx
+++ b/gameData/shared/HouseFunction.xlsx
@@ -51,16 +51,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
-    <t>INT_population</t>
-  </si>
-  <si>
-    <t>INT_poduction</t>
-  </si>
-  <si>
-    <t>INT_poduction</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>INT_level</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -69,6 +59,18 @@
   </si>
   <si>
     <t>INT_recoveryCitizen</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_citizen</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_poduction</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_poduction</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -232,7 +234,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="310">
+  <cellStyleXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -247,6 +249,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -563,7 +569,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="310">
+  <cellStyles count="314">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -721,6 +727,8 @@
     <cellStyle name="超链接" xfId="304" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="306" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="312" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -871,6 +879,8 @@
     <cellStyle name="访问过的超链接" xfId="305" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="307" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="313" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1323,7 +1333,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1333,16 +1343,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -1656,7 +1666,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1666,13 +1676,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -1923,7 +1933,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1933,13 +1943,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -2190,7 +2200,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2200,13 +2210,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -2457,7 +2467,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2467,13 +2477,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">

</xml_diff>